<commit_message>
Add instructions to running tests locally to test_report.
</commit_message>
<xml_diff>
--- a/comp-se-200-assignment-Bug-Reports.xlsx
+++ b/comp-se-200-assignment-Bug-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Software-Testing\comp-se-200-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23838F4-5540-4905-9C36-09615F42EEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB63FF9-7FAE-4E05-BF88-8CD0D17125D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D27F42CA-42A7-437E-AB23-64748E0BB2CF}"/>
   </bookViews>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>otula</t>
-  </si>
-  <si>
-    <t>Function is used to show price information to the user and that is why Seriousness is determined to be critical. Fix should be straightforward to implement.</t>
   </si>
   <si>
     <r>
@@ -170,6 +167,9 @@
       </rPr>
       <t xml:space="preserve"> / divisor on line 16 of divide.js</t>
     </r>
+  </si>
+  <si>
+    <t>Function is used to show price information to the user and that is why Seriousness is determined to be major. Fix should be straightforward to implement.</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +725,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,7 +749,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update bug reports excel by adding a bug report for words.js failing test
</commit_message>
<xml_diff>
--- a/comp-se-200-assignment-Bug-Reports.xlsx
+++ b/comp-se-200-assignment-Bug-Reports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Software-Testing\comp-se-200-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\anxored\c\m\comp-se-200\comp-se-200-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB63FF9-7FAE-4E05-BF88-8CD0D17125D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552134AC-F1E3-4F58-8E08-EB910A9420F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D27F42CA-42A7-437E-AB23-64748E0BB2CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D27F42CA-42A7-437E-AB23-64748E0BB2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Bug report</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>kgolsu</t>
-  </si>
-  <si>
-    <t>xxx</t>
   </si>
   <si>
     <t>Yes</t>
@@ -170,6 +167,32 @@
   </si>
   <si>
     <t>Function is used to show price information to the user and that is why Seriousness is determined to be major. Fix should be straightforward to implement.</t>
+  </si>
+  <si>
+    <t>Locally: npm test</t>
+  </si>
+  <si>
+    <t>petrikreus</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the words function is given a second parameter as a string, the function returns an unexpected array. </t>
+  </si>
+  <si>
+    <t>1. Force the usage with RegExp by throwing an error when a string or number is used as a second parameter.
+2. Check if the second parameter is a string. If it is, escape special characters to avoid unexpected results and return first index of the result array: string.match(pattern)[0].
+See: https://developer.mozilla.org/en-US/docs/Web/JavaScript/Reference/Global_Objects/String/match#a_non-regexp_as_the_parameter</t>
+  </si>
+  <si>
+    <t>Possible programming error in the file words.js, when words() is used with a string parameter. Refers to Test ID TC022</t>
+  </si>
+  <si>
+    <t>Node v16.17.0, Jest 29.1.2, Coveralls 3.1.1, Ubuntu 20.04.5 LTS (WSL2)</t>
+  </si>
+  <si>
+    <t>The main use case of the function is expected to be without the second parameter, or the second parameter being a RegExp. That is the reason for minor seriousness.</t>
   </si>
 </sst>
 </file>
@@ -290,7 +313,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C2E74B-874F-4CAD-802E-F120C83B59B5}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -653,7 +676,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +716,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,7 +740,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -733,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -774,20 +797,20 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -795,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -803,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="8">
-        <v>44909</v>
+        <v>44910</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -811,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -819,7 +842,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -827,7 +850,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -835,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -843,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,15 +874,15 @@
         <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -867,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -878,26 +901,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17 B37" xr:uid="{41A34F0B-B08C-402F-81D1-BF01DACBF26D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17 B37 B57" xr:uid="{41A34F0B-B08C-402F-81D1-BF01DACBF26D}">
       <formula1>"New,Assigned,Fixed,Verified,Re-open,Won't Fix,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B32" xr:uid="{54127AD1-AD0D-4451-9944-0F0E4DA2A4C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B32 B52" xr:uid="{54127AD1-AD0D-4451-9944-0F0E4DA2A4C8}">
       <formula1>"Yes,No,Sometimes,Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13 B33" xr:uid="{62028496-FB14-4512-ACE7-7840C4EB9239}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13 B33 B53" xr:uid="{62028496-FB14-4512-ACE7-7840C4EB9239}">
       <formula1>"Major,Medium,Minor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B31" xr:uid="{5DB42736-7F8C-4E7B-BF72-4C87116786EE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B31 B51" xr:uid="{5DB42736-7F8C-4E7B-BF72-4C87116786EE}">
       <formula1>"Programming error,Design error,Conflict with documentation,Proposal,Question"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update bug reports and test report. Create test report pdf.
</commit_message>
<xml_diff>
--- a/comp-se-200-assignment-Bug-Reports.xlsx
+++ b/comp-se-200-assignment-Bug-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\anxored\c\m\comp-se-200\comp-se-200-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552134AC-F1E3-4F58-8E08-EB910A9420F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECDA7D6-818D-42FF-9BFB-066C78A0325D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D27F42CA-42A7-437E-AB23-64748E0BB2CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Bug report</t>
   </si>
@@ -181,18 +181,31 @@
     <t xml:space="preserve">When the words function is given a second parameter as a string, the function returns an unexpected array. </t>
   </si>
   <si>
+    <t>Node v16.17.0, Jest 29.1.2, Coveralls 3.1.1, Ubuntu 20.04.5 LTS (WSL2)</t>
+  </si>
+  <si>
+    <t>The main use case of the function is expected to be without the second parameter, or the second parameter being a RegExp. That is the reason for minor seriousness.</t>
+  </si>
+  <si>
+    <t>TC001, TC004</t>
+  </si>
+  <si>
+    <t>Related Test ID(s)</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>Design error</t>
+  </si>
+  <si>
     <t>1. Force the usage with RegExp by throwing an error when a string or number is used as a second parameter.
+OR
 2. Check if the second parameter is a string. If it is, escape special characters to avoid unexpected results and return first index of the result array: string.match(pattern)[0].
 See: https://developer.mozilla.org/en-US/docs/Web/JavaScript/Reference/Global_Objects/String/match#a_non-regexp_as_the_parameter</t>
   </si>
   <si>
-    <t>Possible programming error in the file words.js, when words() is used with a string parameter. Refers to Test ID TC022</t>
-  </si>
-  <si>
-    <t>Node v16.17.0, Jest 29.1.2, Coveralls 3.1.1, Ubuntu 20.04.5 LTS (WSL2)</t>
-  </si>
-  <si>
-    <t>The main use case of the function is expected to be without the second parameter, or the second parameter being a RegExp. That is the reason for minor seriousness.</t>
+    <t>Possible design error in the file words.js, when words() is used with a string as a second parameter</t>
   </si>
 </sst>
 </file>
@@ -629,16 +642,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C2E74B-874F-4CAD-802E-F120C83B59B5}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.33203125" customWidth="1"/>
-    <col min="2" max="2" width="74.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -671,256 +684,272 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8">
-        <v>44909</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>44909</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="8">
-        <v>44910</v>
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="B30" s="8">
+        <v>44910</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>38</v>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17 B37 B57" xr:uid="{41A34F0B-B08C-402F-81D1-BF01DACBF26D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 B39 B59" xr:uid="{41A34F0B-B08C-402F-81D1-BF01DACBF26D}">
       <formula1>"New,Assigned,Fixed,Verified,Re-open,Won't Fix,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B32 B52" xr:uid="{54127AD1-AD0D-4451-9944-0F0E4DA2A4C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13 B34 B54" xr:uid="{54127AD1-AD0D-4451-9944-0F0E4DA2A4C8}">
       <formula1>"Yes,No,Sometimes,Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13 B33 B53" xr:uid="{62028496-FB14-4512-ACE7-7840C4EB9239}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14 B35 B55" xr:uid="{62028496-FB14-4512-ACE7-7840C4EB9239}">
       <formula1>"Major,Medium,Minor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B31 B51" xr:uid="{5DB42736-7F8C-4E7B-BF72-4C87116786EE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B33 B53" xr:uid="{5DB42736-7F8C-4E7B-BF72-4C87116786EE}">
       <formula1>"Programming error,Design error,Conflict with documentation,Proposal,Question"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>